<commit_message>
Can loop through clientList to look for items
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCB8E1B-D40C-4E22-92D5-44EED2AD1B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C85A7D-CE78-44F0-9A85-5EC5ADD24D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3570" windowWidth="16800" windowHeight="9670" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1030" yWindow="2070" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -49,19 +49,19 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Trip Total</t>
-  </si>
-  <si>
     <t>Pay</t>
   </si>
   <si>
-    <t>Visted</t>
-  </si>
-  <si>
-    <t>Overall Cost</t>
-  </si>
-  <si>
-    <t>Tax</t>
+    <t>Out of Stock</t>
+  </si>
+  <si>
+    <t>Not in Stores</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -413,20 +413,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9C3CD1-3B91-4AB6-93A9-994EC74062EE}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" customWidth="1"/>
     <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="8" max="8" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,20 +439,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,7 +473,7 @@
     <col min="8" max="8" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,20 +483,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -503,10 +506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +517,7 @@
     <col min="8" max="8" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,20 +527,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote expense report for 1 client visiting 1 store, no vendor tax yet.
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C85A7D-CE78-44F0-9A85-5EC5ADD24D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7508657-6C79-488D-B346-993B25B0954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1030" yWindow="2070" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1370" yWindow="2410" windowWidth="16800" windowHeight="9670" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>In Stock</t>
   </si>
@@ -62,6 +62,27 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Visited</t>
+  </si>
+  <si>
+    <t>Premium Cat Food</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Catnip</t>
+  </si>
+  <si>
+    <t>Body Butter</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
   </si>
 </sst>
 </file>
@@ -413,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9C3CD1-3B91-4AB6-93A9-994EC74062EE}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,7 +450,7 @@
     <col min="8" max="8" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,14 +466,56 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11.99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>11.99</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>31.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -462,18 +525,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
     <col min="8" max="8" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,13 +554,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,18 +574,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,13 +601,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Probably have vendortax and storestovisit working (tested on 1 client to 1 store so far)
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7508657-6C79-488D-B346-993B25B0954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D7FB8F-AFDF-45FB-904C-FDDC85E7D6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1370" yWindow="2410" windowWidth="16800" windowHeight="9670" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1030" yWindow="2070" windowWidth="16800" windowHeight="9670" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Also writes updated vendors (was commented out for testing rest of it)
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544168D6-7AED-4775-B307-34EDA038637F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7276116A-4E1D-4079-AF9C-19D58E24605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1370" yWindow="2410" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1710" yWindow="2750" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>In Stock</t>
   </si>
@@ -575,7 +575,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -627,6 +627,9 @@
       <c r="C2">
         <v>9.99</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
@@ -634,24 +637,24 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>33.97</v>
+        <v>21.98</v>
       </c>
       <c r="J2">
         <v>20.2</v>
       </c>
       <c r="K2">
-        <v>54.17</v>
+        <v>42.18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>11.99</v>
+        <v>4.99</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -659,23 +662,12 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
         <v>7</v>
       </c>
     </row>
@@ -686,7 +678,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:K1"/>
@@ -738,50 +730,34 @@
       <c r="C2">
         <v>11.99</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="I2">
-        <v>32.979999999999997</v>
+        <v>20.98</v>
       </c>
       <c r="J2">
         <v>20</v>
       </c>
       <c r="K2">
-        <v>52.98</v>
+        <v>40.98</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+        <v>8.99</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>8.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can write a ShopsToVisit.txt
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7276116A-4E1D-4079-AF9C-19D58E24605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE5A2E-279D-44FD-9499-7F1DA5D2F90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="2750" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>In Stock</t>
   </si>
@@ -575,7 +575,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -627,9 +627,6 @@
       <c r="C2">
         <v>9.99</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
@@ -637,24 +634,24 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>21.98</v>
+        <v>33.97</v>
       </c>
       <c r="J2">
         <v>20.2</v>
       </c>
       <c r="K2">
-        <v>42.18</v>
+        <v>54.17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>4.99</v>
+        <v>11.99</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -662,12 +659,23 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>7</v>
       </c>
     </row>
@@ -678,7 +686,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:K1"/>
@@ -730,34 +738,50 @@
       <c r="C2">
         <v>11.99</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="I2">
-        <v>20.98</v>
+        <v>32.979999999999997</v>
       </c>
       <c r="J2">
         <v>20</v>
       </c>
       <c r="K2">
-        <v>40.98</v>
+        <v>52.98</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
         <v>8.99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Does not record client3recExpense, works with other 2 and uses same sequence.
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFF9DFC-D110-4E3F-B325-4078F3B850EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B277084A-A543-4FEB-B9ED-3E63466BE549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="2750" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1710" yWindow="2750" windowWidth="16800" windowHeight="9670" activeTab="1" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Can choose store order as well.
</commit_message>
<xml_diff>
--- a/ClientsExpenses.xlsx
+++ b/ClientsExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743BDA06-6B62-4093-8AA7-F6E4B824E84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0C53E0-574F-4924-BA92-3B38DE471226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1370" yWindow="2410" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
+    <workbookView xWindow="1710" yWindow="2750" windowWidth="16800" windowHeight="9670" activeTab="1" xr2:uid="{53918508-9044-4949-BC64-B843A1A90863}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -67,46 +67,46 @@
     <t>Visited</t>
   </si>
   <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Grocery</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Body Butter</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Premium Cat Food</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Catnip</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Basic Dog Food</t>
+  </si>
+  <si>
+    <t>Oatmeal Soap</t>
+  </si>
+  <si>
     <t>Cat Litter</t>
   </si>
   <si>
-    <t>Pet</t>
-  </si>
-  <si>
-    <t>Premium Cat Food</t>
-  </si>
-  <si>
     <t>Brush</t>
   </si>
   <si>
-    <t>Oatmeal Soap</t>
-  </si>
-  <si>
-    <t>Bath</t>
-  </si>
-  <si>
     <t>Cat Bed</t>
-  </si>
-  <si>
-    <t>Body Butter</t>
-  </si>
-  <si>
-    <t>Fruits</t>
-  </si>
-  <si>
-    <t>Grocery</t>
-  </si>
-  <si>
-    <t>Vegetables</t>
-  </si>
-  <si>
-    <t>Catnip</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Basic Dog Food</t>
   </si>
 </sst>
 </file>
@@ -505,16 +505,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>11.99</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -531,41 +531,41 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>11.99</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33B5547-9C84-4FFD-A18A-58C886975D21}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -619,19 +619,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>9.99</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I2">
         <v>33.97</v>
@@ -645,38 +645,38 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>11.99</v>
+        <v>9.99</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>4.99</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>4.99</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0914DE44-216B-4CE9-8DE5-E8C6B7557947}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -730,16 +730,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>11.99</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>32.979999999999997</v>
@@ -753,10 +753,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -764,10 +764,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -775,10 +775,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>8.99</v>

</xml_diff>